<commit_message>
Update project04 - 요구사항 정의서2.xlsx
</commit_message>
<xml_diff>
--- a/2 기능 정의 취합, 요구사항 정의서, USE FLOW/project04 - 요구사항 정의서2.xlsx
+++ b/2 기능 정의 취합, 요구사항 정의서, USE FLOW/project04 - 요구사항 정의서2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HYEONTAE\Desktop\e-Zone\2 기능 정의 취합, 요구사항 정의서, USE FLOW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\507-07\Desktop\e-Zone\2 기능 정의 취합, 요구사항 정의서, USE FLOW\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="21636" windowHeight="11664"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="21630" windowHeight="11670"/>
   </bookViews>
   <sheets>
     <sheet name="요구사항정의서" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">요구사항정의서!$A$7:$O$26</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="117">
   <si>
     <t>요구사항정의서</t>
   </si>
@@ -246,10 +245,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>메인화면 내의 메뉴에서 강연 정보로 이동하여 상세 내용을 확인 가능, 검색, 카테고리를 통해서 특정 강연 검색 가능</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>KB – P - 008</t>
   </si>
   <si>
@@ -404,10 +399,6 @@
   </si>
   <si>
     <t>강연장 정보 확인 페이지에서 해당 강연장 링크를 클릭하여 강연장 예약 가능, 날짜 선택, 시간대 선택하여 예약 및 결제, 결제 상태 확인</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>강연 정보를 확인하는 페이지에서 강연 정보를 확인한 후, 인원 수, 좌석을 선택한 후 예약 및 결제, 결제 상태 확인</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
@@ -524,11 +515,43 @@
     <t>세미나게스트</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
+  <si>
+    <t>메인화면 내의 메뉴에서 강연 정보로 이동하여 상세 내용을 확인 가능, 검색, 카테고리를 통해서 특정 강연 검색 가능</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>강연 정보를 확인하는 페이지에서 강연 정보를 확인한 후, 인원 수, 좌석을 선택한 후 예약 및 결제, 결제 상태 확인</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>서희</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>서희</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>서희</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>서희</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>현태</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>현태</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -1031,27 +1054,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1073,19 +1075,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1094,25 +1105,37 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1332,24 +1355,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF990"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B12"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.2" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
-    <col min="3" max="3" width="38.44140625" customWidth="1"/>
-    <col min="4" max="4" width="87.5546875" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" customWidth="1"/>
+    <col min="4" max="4" width="87.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="24.109375" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="18.109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="24.140625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="44" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" hidden="1" customWidth="1"/>
     <col min="14" max="15" width="20" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1389,21 +1412,21 @@
     </row>
     <row r="2" spans="1:32" ht="19.5" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="50"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="71"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -1425,19 +1448,19 @@
     </row>
     <row r="3" spans="1:32" ht="19.5" customHeight="1" thickBot="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="51"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="53"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="73"/>
+      <c r="N3" s="74"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -1582,12 +1605,12 @@
       <c r="F7" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="54" t="s">
+      <c r="G7" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="54"/>
-      <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
+      <c r="H7" s="75"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="75"/>
       <c r="K7" s="37" t="s">
         <v>9</v>
       </c>
@@ -1621,18 +1644,18 @@
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
     </row>
-    <row r="8" spans="1:32" ht="33.15" customHeight="1">
+    <row r="8" spans="1:32" ht="33.200000000000003" customHeight="1">
       <c r="A8" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="63"/>
-      <c r="D8" s="64" t="s">
+      <c r="C8" s="68"/>
+      <c r="D8" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="55"/>
+      <c r="E8" s="48"/>
       <c r="F8" s="18"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
@@ -1667,18 +1690,18 @@
       <c r="AE8" s="1"/>
       <c r="AF8" s="1"/>
     </row>
-    <row r="9" spans="1:32" ht="33.15" customHeight="1">
+    <row r="9" spans="1:32" ht="33.200000000000003" customHeight="1">
       <c r="A9" s="62"/>
       <c r="B9" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="66" t="s">
+      <c r="C9" s="56" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="55"/>
+      <c r="E9" s="48"/>
       <c r="F9" s="18"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
@@ -1713,16 +1736,16 @@
       <c r="AE9" s="1"/>
       <c r="AF9" s="1"/>
     </row>
-    <row r="10" spans="1:32" ht="33.15" customHeight="1">
+    <row r="10" spans="1:32" ht="33.200000000000003" customHeight="1">
       <c r="A10" s="62"/>
       <c r="B10" s="65"/>
       <c r="C10" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="64" t="s">
+      <c r="D10" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="56"/>
+      <c r="E10" s="49"/>
       <c r="F10" s="7"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
@@ -1763,10 +1786,10 @@
       <c r="C11" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="56"/>
+      <c r="E11" s="49"/>
       <c r="F11" s="7"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -1807,10 +1830,10 @@
       <c r="C12" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="64" t="s">
+      <c r="D12" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="56"/>
+      <c r="E12" s="49"/>
       <c r="F12" s="7"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
@@ -1839,18 +1862,18 @@
       <c r="AE12" s="1"/>
       <c r="AF12" s="1"/>
     </row>
-    <row r="13" spans="1:32" ht="33.15" customHeight="1">
+    <row r="13" spans="1:32" ht="33.200000000000003" customHeight="1">
       <c r="A13" s="62"/>
-      <c r="B13" s="67" t="s">
+      <c r="B13" s="63" t="s">
         <v>32</v>
       </c>
       <c r="C13" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="64" t="s">
+      <c r="D13" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="56"/>
+      <c r="E13" s="49"/>
       <c r="F13" s="7"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -1885,16 +1908,16 @@
       <c r="AE13" s="1"/>
       <c r="AF13" s="1"/>
     </row>
-    <row r="14" spans="1:32" ht="33.15" customHeight="1">
+    <row r="14" spans="1:32" ht="33.200000000000003" customHeight="1">
       <c r="A14" s="62"/>
-      <c r="B14" s="67"/>
+      <c r="B14" s="63"/>
       <c r="C14" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="64" t="s">
+      <c r="D14" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="56"/>
+      <c r="E14" s="49"/>
       <c r="F14" s="7"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
@@ -1923,16 +1946,16 @@
       <c r="AE14" s="1"/>
       <c r="AF14" s="1"/>
     </row>
-    <row r="15" spans="1:32" ht="33.15" customHeight="1">
+    <row r="15" spans="1:32" ht="33.200000000000003" customHeight="1">
       <c r="A15" s="62"/>
-      <c r="B15" s="67"/>
+      <c r="B15" s="63"/>
       <c r="C15" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="64" t="s">
-        <v>87</v>
-      </c>
-      <c r="E15" s="56"/>
+      <c r="D15" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="49"/>
       <c r="F15" s="7"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -1961,16 +1984,16 @@
       <c r="AE15" s="1"/>
       <c r="AF15" s="1"/>
     </row>
-    <row r="16" spans="1:32" ht="33.15" customHeight="1">
+    <row r="16" spans="1:32" ht="33.200000000000003" customHeight="1">
       <c r="A16" s="62"/>
-      <c r="B16" s="67"/>
+      <c r="B16" s="63"/>
       <c r="C16" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="64" t="s">
-        <v>86</v>
-      </c>
-      <c r="E16" s="56"/>
+      <c r="D16" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="49"/>
       <c r="F16" s="7"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
@@ -1999,19 +2022,21 @@
       <c r="AE16" s="1"/>
       <c r="AF16" s="1"/>
     </row>
-    <row r="17" spans="1:32" ht="33.15" customHeight="1">
+    <row r="17" spans="1:32" ht="33.200000000000003" customHeight="1">
       <c r="A17" s="62"/>
-      <c r="B17" s="68" t="s">
+      <c r="B17" s="64" t="s">
         <v>41</v>
       </c>
       <c r="C17" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="69" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="56"/>
-      <c r="F17" s="7"/>
+      <c r="D17" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" s="49"/>
+      <c r="F17" s="7" t="s">
+        <v>111</v>
+      </c>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
@@ -2022,10 +2047,10 @@
         <v>1</v>
       </c>
       <c r="N17" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="O17" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="O17" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
@@ -2047,15 +2072,17 @@
     </row>
     <row r="18" spans="1:32" ht="33.6" customHeight="1">
       <c r="A18" s="62"/>
-      <c r="B18" s="68"/>
+      <c r="B18" s="64"/>
       <c r="C18" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="69" t="s">
-        <v>88</v>
-      </c>
-      <c r="E18" s="56"/>
-      <c r="F18" s="7"/>
+        <v>45</v>
+      </c>
+      <c r="D18" s="57" t="s">
+        <v>110</v>
+      </c>
+      <c r="E18" s="49"/>
+      <c r="F18" s="7" t="s">
+        <v>112</v>
+      </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="33"/>
@@ -2066,10 +2093,10 @@
         <v>2</v>
       </c>
       <c r="N18" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="O18" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="O18" s="5" t="s">
-        <v>48</v>
       </c>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
@@ -2089,17 +2116,19 @@
       <c r="AE18" s="1"/>
       <c r="AF18" s="1"/>
     </row>
-    <row r="19" spans="1:32" ht="28.8" customHeight="1">
+    <row r="19" spans="1:32" ht="28.9" customHeight="1">
       <c r="A19" s="62"/>
-      <c r="B19" s="68"/>
+      <c r="B19" s="64"/>
       <c r="C19" s="44" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D19" s="45" t="s">
-        <v>97</v>
-      </c>
-      <c r="E19" s="57"/>
-      <c r="F19" s="16"/>
+        <v>95</v>
+      </c>
+      <c r="E19" s="50"/>
+      <c r="F19" s="16" t="s">
+        <v>113</v>
+      </c>
       <c r="G19" s="26"/>
       <c r="H19" s="26"/>
       <c r="I19" s="26"/>
@@ -2110,10 +2139,10 @@
         <v>1</v>
       </c>
       <c r="N19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="O19" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="O19" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
@@ -2133,17 +2162,19 @@
       <c r="AE19" s="1"/>
       <c r="AF19" s="1"/>
     </row>
-    <row r="20" spans="1:32" ht="28.8" customHeight="1">
+    <row r="20" spans="1:32" ht="28.9" customHeight="1">
       <c r="A20" s="62"/>
-      <c r="B20" s="68"/>
+      <c r="B20" s="64"/>
       <c r="C20" s="44" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D20" s="45" t="s">
-        <v>99</v>
-      </c>
-      <c r="E20" s="57"/>
-      <c r="F20" s="16"/>
+        <v>97</v>
+      </c>
+      <c r="E20" s="50"/>
+      <c r="F20" s="16" t="s">
+        <v>112</v>
+      </c>
       <c r="G20" s="26"/>
       <c r="H20" s="26"/>
       <c r="I20" s="33"/>
@@ -2154,10 +2185,10 @@
         <v>2</v>
       </c>
       <c r="N20" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="O20" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="O20" s="5" t="s">
-        <v>48</v>
       </c>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
@@ -2177,17 +2208,19 @@
       <c r="AE20" s="1"/>
       <c r="AF20" s="1"/>
     </row>
-    <row r="21" spans="1:32" ht="28.8" customHeight="1">
+    <row r="21" spans="1:32" ht="28.9" customHeight="1">
       <c r="A21" s="62"/>
-      <c r="B21" s="68"/>
+      <c r="B21" s="64"/>
       <c r="C21" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="69" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21" s="56"/>
-      <c r="F21" s="7"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="7" t="s">
+        <v>114</v>
+      </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="34"/>
@@ -2215,19 +2248,21 @@
       <c r="AE21" s="1"/>
       <c r="AF21" s="1"/>
     </row>
-    <row r="22" spans="1:32" ht="28.8" customHeight="1">
+    <row r="22" spans="1:32" ht="28.9" customHeight="1">
       <c r="A22" s="62"/>
-      <c r="B22" s="70" t="s">
+      <c r="B22" s="67" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="43" t="s">
+      <c r="D22" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="69" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" s="58"/>
-      <c r="F22" s="12"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="12" t="s">
+        <v>115</v>
+      </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
@@ -2238,10 +2273,10 @@
         <v>1</v>
       </c>
       <c r="N22" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="O22" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="O22" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
@@ -2261,17 +2296,19 @@
       <c r="AE22" s="1"/>
       <c r="AF22" s="1"/>
     </row>
-    <row r="23" spans="1:32" ht="33.15" customHeight="1">
+    <row r="23" spans="1:32" ht="33.200000000000003" customHeight="1">
       <c r="A23" s="62"/>
-      <c r="B23" s="70"/>
+      <c r="B23" s="67"/>
       <c r="C23" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="44" t="s">
-        <v>57</v>
-      </c>
-      <c r="E23" s="58"/>
-      <c r="F23" s="12"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="12" t="s">
+        <v>74</v>
+      </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
@@ -2282,10 +2319,10 @@
         <v>2</v>
       </c>
       <c r="N23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="O23" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="O23" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
@@ -2305,20 +2342,20 @@
       <c r="AE23" s="1"/>
       <c r="AF23" s="1"/>
     </row>
-    <row r="24" spans="1:32" ht="33.15" customHeight="1">
+    <row r="24" spans="1:32" ht="33.200000000000003" customHeight="1">
       <c r="A24" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="71" t="s">
+      <c r="C24" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="47" t="s">
+      <c r="D24" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="D24" s="46" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" s="59"/>
+      <c r="E24" s="52"/>
       <c r="F24" s="35"/>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
@@ -2347,18 +2384,18 @@
       <c r="AE24" s="1"/>
       <c r="AF24" s="1"/>
     </row>
-    <row r="25" spans="1:32" ht="33.15" customHeight="1">
+    <row r="25" spans="1:32" ht="33.200000000000003" customHeight="1">
       <c r="A25" s="62"/>
       <c r="B25" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" s="47" t="s">
-        <v>65</v>
-      </c>
-      <c r="E25" s="60"/>
+      <c r="E25" s="53"/>
       <c r="F25" s="24"/>
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
@@ -2370,7 +2407,7 @@
         <v>3</v>
       </c>
       <c r="N25" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O25" s="5"/>
       <c r="P25" s="1"/>
@@ -2391,18 +2428,18 @@
       <c r="AE25" s="1"/>
       <c r="AF25" s="1"/>
     </row>
-    <row r="26" spans="1:32" ht="33.15" customHeight="1">
+    <row r="26" spans="1:32" ht="33.200000000000003" customHeight="1">
       <c r="A26" s="62"/>
       <c r="B26" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26" s="72" t="s">
-        <v>68</v>
-      </c>
-      <c r="E26" s="56"/>
+      <c r="E26" s="49"/>
       <c r="F26" s="7"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -2414,7 +2451,7 @@
         <v>3</v>
       </c>
       <c r="N26" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O26" s="3"/>
       <c r="P26" s="1"/>
@@ -2435,19 +2472,21 @@
       <c r="AE26" s="1"/>
       <c r="AF26" s="1"/>
     </row>
-    <row r="27" spans="1:32" ht="33.15" customHeight="1">
+    <row r="27" spans="1:32" ht="33.200000000000003" customHeight="1">
       <c r="A27" s="62"/>
-      <c r="B27" s="73" t="s">
+      <c r="B27" s="61" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="C27" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="E27" s="61"/>
-      <c r="F27" s="17"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="17" t="s">
+        <v>116</v>
+      </c>
       <c r="G27" s="17"/>
       <c r="H27" s="17"/>
       <c r="I27" s="17"/>
@@ -2475,17 +2514,19 @@
       <c r="AE27" s="1"/>
       <c r="AF27" s="1"/>
     </row>
-    <row r="28" spans="1:32" ht="33.15" customHeight="1">
+    <row r="28" spans="1:32" ht="33.200000000000003" customHeight="1">
       <c r="A28" s="62"/>
-      <c r="B28" s="73"/>
+      <c r="B28" s="61"/>
       <c r="C28" s="43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D28" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="E28" s="61"/>
-      <c r="F28" s="17"/>
+        <v>71</v>
+      </c>
+      <c r="E28" s="54"/>
+      <c r="F28" s="17" t="s">
+        <v>116</v>
+      </c>
       <c r="G28" s="17"/>
       <c r="H28" s="17"/>
       <c r="I28" s="17"/>
@@ -2515,14 +2556,14 @@
     </row>
     <row r="29" spans="1:32" ht="45.75" customHeight="1">
       <c r="A29" s="62"/>
-      <c r="B29" s="74" t="s">
-        <v>94</v>
+      <c r="B29" s="66" t="s">
+        <v>92</v>
       </c>
       <c r="C29" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="60" t="s">
         <v>73</v>
-      </c>
-      <c r="D29" s="75" t="s">
-        <v>74</v>
       </c>
       <c r="E29" s="2"/>
       <c r="G29" s="1"/>
@@ -2552,12 +2593,12 @@
     </row>
     <row r="30" spans="1:32" ht="44.1" customHeight="1">
       <c r="A30" s="62"/>
-      <c r="B30" s="74"/>
+      <c r="B30" s="66"/>
       <c r="C30" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="D30" s="60" t="s">
         <v>89</v>
-      </c>
-      <c r="D30" s="75" t="s">
-        <v>91</v>
       </c>
       <c r="E30" s="2"/>
       <c r="G30" s="1"/>
@@ -2588,16 +2629,18 @@
     <row r="31" spans="1:32" ht="52.5" customHeight="1">
       <c r="A31" s="62"/>
       <c r="B31" s="44" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C31" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="D31" s="44" t="s">
-        <v>92</v>
-      </c>
       <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
+      <c r="F31" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -2661,7 +2704,7 @@
       <c r="B33" s="2"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
@@ -2669,7 +2712,7 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="1"/>
@@ -2697,7 +2740,7 @@
     <row r="34" spans="1:32" ht="15.75" customHeight="1">
       <c r="A34" s="1"/>
       <c r="D34" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -2705,7 +2748,7 @@
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K34" s="2"/>
       <c r="L34" s="1"/>
@@ -2739,7 +2782,7 @@
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K35" s="2"/>
       <c r="L35" s="1"/>
@@ -2773,7 +2816,7 @@
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K36" s="2"/>
       <c r="L36" s="1"/>
@@ -2807,7 +2850,7 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K37" s="2"/>
       <c r="L37" s="1"/>
@@ -2902,7 +2945,7 @@
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="C40" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="2"/>
@@ -2937,10 +2980,10 @@
     <row r="41" spans="1:32" ht="15.75" customHeight="1">
       <c r="A41" s="1"/>
       <c r="B41" s="42" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="2"/>
@@ -2975,10 +3018,10 @@
     <row r="42" spans="1:32" ht="15.75" customHeight="1">
       <c r="A42" s="1"/>
       <c r="B42" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="2"/>
@@ -3013,10 +3056,10 @@
     <row r="43" spans="1:32" ht="15.75" customHeight="1">
       <c r="A43" s="1"/>
       <c r="B43" s="41" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="2"/>
@@ -3051,10 +3094,10 @@
     <row r="44" spans="1:32" ht="15.75" customHeight="1">
       <c r="A44" s="1"/>
       <c r="B44" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="2"/>
@@ -3089,10 +3132,10 @@
     <row r="45" spans="1:32" ht="15.75" customHeight="1">
       <c r="A45" s="1"/>
       <c r="B45" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="2"/>
@@ -10148,6 +10191,8 @@
     <filterColumn colId="9" hiddenButton="1" showButton="0"/>
   </autoFilter>
   <mergeCells count="11">
+    <mergeCell ref="B2:N3"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="A8:A23"/>
     <mergeCell ref="B13:B16"/>
@@ -10157,8 +10202,6 @@
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B2:N3"/>
-    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -10177,51 +10220,51 @@
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.2" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="14.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.44140625" customWidth="1"/>
+    <col min="1" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="13.2">
+    <row r="2" spans="2:3" ht="12.75">
       <c r="B2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="12.75">
+      <c r="B3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="13.2">
-      <c r="B3" s="1" t="s">
+    <row r="4" spans="2:3" ht="12.75">
+      <c r="B4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="13.2">
-      <c r="B4" s="1" t="s">
+    <row r="5" spans="2:3" ht="12.75">
+      <c r="B5" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="13.2">
-      <c r="B5" s="1" t="s">
+    <row r="6" spans="2:3" ht="12.75">
+      <c r="B6" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="13.2">
-      <c r="B6" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>